<commit_message>
Results from December_05,_2020--22:02:44 run
</commit_message>
<xml_diff>
--- a/workflow/python/output/xlsx/covid_disparities_output_2020-12-05.xlsx
+++ b/workflow/python/output/xlsx/covid_disparities_output_2020-12-05.xlsx
@@ -211,16 +211,16 @@
     <t>Kentucky</t>
   </si>
   <si>
-    <t>2020-12-04</t>
-  </si>
-  <si>
-    <t>209170</t>
-  </si>
-  <si>
-    <t>925</t>
-  </si>
-  <si>
-    <t>3032</t>
+    <t>2020-12-05</t>
+  </si>
+  <si>
+    <t>212844</t>
+  </si>
+  <si>
+    <t>939</t>
+  </si>
+  <si>
+    <t>3078</t>
   </si>
   <si>
     <t>11</t>
@@ -274,7 +274,7 @@
     <t>An error occurred. ... NoSuchElementException('no such element: Unable to locate element: {"method":"xpath","selector":"//a[@data-chart-id=\'count-charts\']"}\n  (Session info: headless chrome=87.0.4280.88)', None, None)</t>
   </si>
   <si>
-    <t>An error occurred. ... CalledProcessError(1, ['java', '-Djava.awt.headless=true', '-Dfile.encoding=UTF8', '-jar', '/Users/poisson/Documents/GitHub/COVID19_tracker_data_extraction/covid19_data_test_003/lib/python3.7/site-packages/tabula/tabula-1.0.3-jar-with-dependencies.jar', '--pages', '3', '--area', '626.8578491210938,80.14600372314453,961.4368286132812,941.5399780273438', '--stream', '/var/folders/cn/4q_jgh710l170_p6btg_ym880000gn/T/a194c8db-c530-48e2-b03e-fdc6ee882021.pdf'])</t>
+    <t>An error occurred. ... CalledProcessError(1, ['java', '-Djava.awt.headless=true', '-Dfile.encoding=UTF8', '-jar', '/Users/poisson/Documents/GitHub/COVID19_tracker_data_extraction/covid19_data_test_003/lib/python3.7/site-packages/tabula/tabula-1.0.3-jar-with-dependencies.jar', '--pages', '3', '--area', '626.8578491210938,80.14600372314453,961.4368286132812,941.5399780273438', '--stream', '/var/folders/cn/4q_jgh710l170_p6btg_ym880000gn/T/a79b4226-8bf5-4467-b1e6-407a997a8bdd.pdf'])</t>
   </si>
   <si>
     <t>An error occurred. ... ValueError("time data 'Nov-1-2020' does not match format '%B-%d-%Y'")</t>
@@ -705,25 +705,25 @@
         <v>15</v>
       </c>
       <c r="B2" s="2">
-        <v>44169</v>
+        <v>44170</v>
       </c>
       <c r="C2">
-        <v>770088</v>
+        <v>779975</v>
       </c>
       <c r="D2">
-        <v>12974</v>
+        <v>13179</v>
       </c>
       <c r="E2">
-        <v>72012</v>
+        <v>72772</v>
       </c>
       <c r="F2">
-        <v>2659</v>
+        <v>2687</v>
       </c>
       <c r="G2">
-        <v>9.35</v>
+        <v>9.33</v>
       </c>
       <c r="H2">
-        <v>20.49</v>
+        <v>20.39</v>
       </c>
       <c r="I2" t="b">
         <v>1</v>
@@ -769,22 +769,22 @@
         <v>44169</v>
       </c>
       <c r="C4">
-        <v>174290</v>
+        <v>175793</v>
       </c>
       <c r="D4">
         <v>2925</v>
       </c>
       <c r="E4">
-        <v>6183</v>
+        <v>6253</v>
       </c>
       <c r="F4">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="G4">
-        <v>5.89</v>
+        <v>5.84</v>
       </c>
       <c r="H4">
-        <v>3.07</v>
+        <v>3.1</v>
       </c>
       <c r="I4" t="b">
         <v>0</v>
@@ -793,10 +793,10 @@
         <v>0</v>
       </c>
       <c r="K4">
-        <v>104967</v>
+        <v>106997</v>
       </c>
       <c r="L4">
-        <v>2862</v>
+        <v>2875</v>
       </c>
       <c r="M4">
         <v>269854</v>
@@ -813,25 +813,25 @@
         <v>18</v>
       </c>
       <c r="B5" s="2">
-        <v>44169</v>
+        <v>44170</v>
       </c>
       <c r="C5">
-        <v>382534</v>
+        <v>388552</v>
       </c>
       <c r="D5">
-        <v>5467</v>
+        <v>5516</v>
       </c>
       <c r="E5">
-        <v>68514</v>
+        <v>69499</v>
       </c>
       <c r="F5">
-        <v>1466</v>
+        <v>1476</v>
       </c>
       <c r="G5">
-        <v>21.76</v>
+        <v>21.72</v>
       </c>
       <c r="H5">
-        <v>28.11</v>
+        <v>28.03</v>
       </c>
       <c r="I5" t="b">
         <v>0</v>
@@ -840,10 +840,10 @@
         <v>1</v>
       </c>
       <c r="K5">
-        <v>314914</v>
+        <v>320018</v>
       </c>
       <c r="L5">
-        <v>5216</v>
+        <v>5266</v>
       </c>
       <c r="M5">
         <v>2179622</v>
@@ -995,25 +995,25 @@
         <v>25</v>
       </c>
       <c r="B12" s="2">
-        <v>44169</v>
+        <v>44170</v>
       </c>
       <c r="C12">
-        <v>392608</v>
+        <v>397522</v>
       </c>
       <c r="D12">
-        <v>4876</v>
+        <v>4905</v>
       </c>
       <c r="E12">
-        <v>55816</v>
+        <v>56328</v>
       </c>
       <c r="F12">
-        <v>1013</v>
+        <v>1017</v>
       </c>
       <c r="G12">
-        <v>14.22</v>
+        <v>14.17</v>
       </c>
       <c r="H12">
-        <v>20.78</v>
+        <v>20.73</v>
       </c>
       <c r="I12" t="b">
         <v>1</v>
@@ -1150,25 +1150,25 @@
         <v>29</v>
       </c>
       <c r="B16" s="2">
-        <v>44169</v>
+        <v>44170</v>
       </c>
       <c r="C16">
-        <v>167137</v>
+        <v>169382</v>
       </c>
       <c r="D16">
-        <v>2586</v>
+        <v>2620</v>
       </c>
       <c r="E16">
-        <v>29666</v>
+        <v>29954</v>
       </c>
       <c r="F16">
-        <v>424</v>
+        <v>428</v>
       </c>
       <c r="G16">
-        <v>20.06</v>
+        <v>20.03</v>
       </c>
       <c r="H16">
-        <v>17.43</v>
+        <v>17.4</v>
       </c>
       <c r="I16" t="b">
         <v>0</v>
@@ -1177,10 +1177,10 @@
         <v>1</v>
       </c>
       <c r="K16">
-        <v>147873</v>
+        <v>149579</v>
       </c>
       <c r="L16">
-        <v>2432</v>
+        <v>2460</v>
       </c>
       <c r="M16">
         <v>460970</v>
@@ -1258,25 +1258,25 @@
         <v>32</v>
       </c>
       <c r="B19" s="2">
-        <v>44169</v>
+        <v>44170</v>
       </c>
       <c r="C19">
-        <v>388961</v>
+        <v>394976</v>
       </c>
       <c r="D19">
-        <v>9606</v>
+        <v>9797</v>
       </c>
       <c r="E19">
-        <v>44878</v>
+        <v>45609</v>
       </c>
       <c r="F19">
-        <v>2768</v>
+        <v>2780</v>
       </c>
       <c r="G19">
-        <v>11.54</v>
+        <v>11.55</v>
       </c>
       <c r="H19">
-        <v>28.82</v>
+        <v>28.38</v>
       </c>
       <c r="I19" t="b">
         <v>1</v>
@@ -1322,22 +1322,22 @@
         <v>65</v>
       </c>
       <c r="C21">
-        <v>208875</v>
+        <v>213245</v>
       </c>
       <c r="D21">
-        <v>1860</v>
+        <v>1874</v>
       </c>
       <c r="E21">
-        <v>12574.275</v>
+        <v>12773.3755</v>
       </c>
       <c r="F21">
-        <v>111.042</v>
+        <v>113.0022</v>
       </c>
       <c r="G21">
-        <v>6.02</v>
+        <v>5.99</v>
       </c>
       <c r="H21">
-        <v>5.97</v>
+        <v>6.03</v>
       </c>
       <c r="I21" t="b">
         <v>0</v>
@@ -1346,10 +1346,10 @@
         <v>0</v>
       </c>
       <c r="K21">
-        <v>163361.1375</v>
+        <v>166331.1</v>
       </c>
       <c r="L21">
-        <v>1702.086</v>
+        <v>1716.0218</v>
       </c>
       <c r="M21">
         <v>287959</v>
@@ -1406,25 +1406,25 @@
         <v>37</v>
       </c>
       <c r="B24" s="2">
-        <v>44169</v>
+        <v>44170</v>
       </c>
       <c r="C24">
-        <v>27196</v>
+        <v>27861</v>
       </c>
       <c r="D24">
-        <v>133</v>
+        <v>141</v>
       </c>
       <c r="E24">
-        <v>930</v>
+        <v>943</v>
       </c>
       <c r="F24">
         <v>6</v>
       </c>
       <c r="G24">
-        <v>3.47</v>
+        <v>3.44</v>
       </c>
       <c r="H24">
-        <v>4.51</v>
+        <v>4.26</v>
       </c>
       <c r="I24" t="b">
         <v>0</v>
@@ -1433,10 +1433,10 @@
         <v>1</v>
       </c>
       <c r="K24">
-        <v>26779</v>
+        <v>27429</v>
       </c>
       <c r="L24">
-        <v>133</v>
+        <v>141</v>
       </c>
       <c r="M24">
         <v>24129</v>
@@ -1490,19 +1490,19 @@
         <v>44170</v>
       </c>
       <c r="C27">
-        <v>242062</v>
+        <v>243384</v>
       </c>
       <c r="D27">
-        <v>2665</v>
+        <v>2666</v>
       </c>
       <c r="E27">
-        <v>8149</v>
+        <v>8162</v>
       </c>
       <c r="F27">
         <v>72</v>
       </c>
       <c r="G27">
-        <v>3.37</v>
+        <v>3.35</v>
       </c>
       <c r="H27">
         <v>2.7</v>
@@ -1548,7 +1548,7 @@
         <v>42</v>
       </c>
       <c r="B29" s="2">
-        <v>44169</v>
+        <v>44170</v>
       </c>
       <c r="C29" t="s">
         <v>66</v>
@@ -1566,7 +1566,7 @@
         <v>1.4</v>
       </c>
       <c r="H29">
-        <v>1.19</v>
+        <v>1.17</v>
       </c>
       <c r="I29" t="b">
         <v>1</v>
@@ -1710,13 +1710,13 @@
         <v>48</v>
       </c>
       <c r="B35" s="2">
-        <v>44169</v>
+        <v>44170</v>
       </c>
       <c r="C35">
-        <v>136325</v>
+        <v>138568</v>
       </c>
       <c r="D35">
-        <v>1186</v>
+        <v>1194</v>
       </c>
       <c r="E35">
         <v>3462</v>
@@ -1757,25 +1757,25 @@
         <v>49</v>
       </c>
       <c r="B36" s="3">
-        <v>44168</v>
+        <v>44169</v>
       </c>
       <c r="C36">
-        <v>1286557</v>
+        <v>1311625</v>
       </c>
       <c r="D36">
-        <v>19582</v>
+        <v>19791</v>
       </c>
       <c r="E36">
-        <v>38137</v>
+        <v>38841</v>
       </c>
       <c r="F36">
-        <v>1414</v>
+        <v>1418</v>
       </c>
       <c r="G36">
         <v>4.1</v>
       </c>
       <c r="H36">
-        <v>7.26</v>
+        <v>7.23</v>
       </c>
       <c r="I36" t="b">
         <v>0</v>
@@ -1784,10 +1784,10 @@
         <v>0</v>
       </c>
       <c r="K36">
-        <v>929184</v>
+        <v>947773</v>
       </c>
       <c r="L36">
-        <v>19481</v>
+        <v>19602</v>
       </c>
       <c r="M36">
         <v>2267875</v>
@@ -1865,16 +1865,16 @@
         <v>52</v>
       </c>
       <c r="B39" s="2">
-        <v>44169</v>
+        <v>44170</v>
       </c>
       <c r="C39">
-        <v>104935</v>
+        <v>106856</v>
       </c>
       <c r="D39">
-        <v>1706</v>
+        <v>1738</v>
       </c>
       <c r="E39">
-        <v>1294</v>
+        <v>1312</v>
       </c>
       <c r="G39">
         <v>1.23</v>
@@ -1940,25 +1940,25 @@
         <v>55</v>
       </c>
       <c r="B42" s="2">
-        <v>44169</v>
+        <v>44170</v>
       </c>
       <c r="C42">
-        <v>252222</v>
+        <v>257347</v>
       </c>
       <c r="D42">
-        <v>3338</v>
+        <v>3357</v>
       </c>
       <c r="E42">
-        <v>6104</v>
+        <v>6202</v>
       </c>
       <c r="F42">
         <v>150</v>
       </c>
       <c r="G42">
-        <v>3.55</v>
+        <v>3.54</v>
       </c>
       <c r="H42">
-        <v>4.78</v>
+        <v>4.75</v>
       </c>
       <c r="I42" t="b">
         <v>0</v>
@@ -1967,10 +1967,10 @@
         <v>0</v>
       </c>
       <c r="K42">
-        <v>172041</v>
+        <v>175279</v>
       </c>
       <c r="L42">
-        <v>3140</v>
+        <v>3157</v>
       </c>
       <c r="M42">
         <v>227938</v>
@@ -2149,25 +2149,25 @@
         <v>62</v>
       </c>
       <c r="B49" s="2">
-        <v>44169</v>
+        <v>44170</v>
       </c>
       <c r="C49">
-        <v>367329</v>
+        <v>375019</v>
       </c>
       <c r="D49">
-        <v>5832</v>
+        <v>5910</v>
       </c>
       <c r="E49">
-        <v>24789</v>
+        <v>25137</v>
       </c>
       <c r="F49">
-        <v>565</v>
+        <v>569</v>
       </c>
       <c r="G49">
-        <v>6.75</v>
+        <v>6.7</v>
       </c>
       <c r="H49">
-        <v>9.69</v>
+        <v>9.630000000000001</v>
       </c>
       <c r="I49" t="b">
         <v>1</v>

</xml_diff>